<commit_message>
Clase 16 de redes
</commit_message>
<xml_diff>
--- a/Clase_11_Maquinas_Virtuales/Triviño_David/Ejercicio de algoritmos de planificación - Práctica.xlsx
+++ b/Clase_11_Maquinas_Virtuales/Triviño_David/Ejercicio de algoritmos de planificación - Práctica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Google Drive\CTD\Introducción a la Informática\camada8_roberto\Clase_11_Maquinas_Virtuales\Triviño_David\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE35DDB4-8E9B-483B-8910-56F9039878B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB56B6-407E-4ACC-BA61-3E61915BA0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIFO" sheetId="1" r:id="rId1"/>
@@ -1636,7 +1636,7 @@
   </sheetPr>
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -2502,7 +2502,7 @@
   </sheetPr>
   <dimension ref="A1:BB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -23975,7 +23975,7 @@
   </sheetPr>
   <dimension ref="A1:BB35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>

</xml_diff>